<commit_message>
aggiunti metodi get e add
</commit_message>
<xml_diff>
--- a/Registri/Riepilogo_Spese_Edo.xlsx
+++ b/Registri/Riepilogo_Spese_Edo.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smartblue-my.sharepoint.com/personal/edoardo_alviti_smartblue_it/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edoal\PycharmProjects\RegistroSpese\Registri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DD38D1B-540C-49A2-B20F-BEF7A86A13AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86437FDD-9AC3-4C65-87C5-20534AB11546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B18A4B1-6C56-4B7F-AFAE-3741FBA4F12E}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="30960" windowHeight="12120" xr2:uid="{3B18A4B1-6C56-4B7F-AFAE-3741FBA4F12E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio2" sheetId="2" r:id="rId1"/>
+    <sheet name="2025" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -180,7 +180,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -699,25 +699,25 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -755,7 +755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:15">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -778,7 +778,7 @@
         <v>420.63</v>
       </c>
       <c r="J2">
-        <f>H2+I2-D17</f>
+        <f t="shared" ref="J2:J13" si="1">H2+I2-D17</f>
         <v>815.34000000000026</v>
       </c>
       <c r="M2" s="4">
@@ -789,7 +789,7 @@
         <v>-43.56</v>
       </c>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>11</v>
       </c>
@@ -811,7 +811,7 @@
         <v>400</v>
       </c>
       <c r="J3">
-        <f>H3+I3-D18</f>
+        <f t="shared" si="1"/>
         <v>695.33999999999992</v>
       </c>
       <c r="M3" s="4">
@@ -826,7 +826,7 @@
         <v>361.10000000000008</v>
       </c>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -848,14 +848,14 @@
         <v>400</v>
       </c>
       <c r="J4">
-        <f>H4+I4-D19</f>
+        <f t="shared" si="1"/>
         <v>757.25</v>
       </c>
       <c r="M4" s="4">
         <v>45755</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N13" si="1">D4-H4+N3</f>
+        <f t="shared" ref="N4:N13" si="2">D4-H4+N3</f>
         <v>1728.8500000000001</v>
       </c>
       <c r="O4">
@@ -863,7 +863,7 @@
         <v>1003.8500000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>13</v>
       </c>
@@ -885,22 +885,22 @@
         <v>450</v>
       </c>
       <c r="J5">
-        <f>H5+I5-D20</f>
+        <f t="shared" si="1"/>
         <v>807.25</v>
       </c>
       <c r="M5" s="4">
         <v>45785</v>
       </c>
       <c r="N5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2771.6000000000004</v>
       </c>
       <c r="O5">
-        <f t="shared" ref="O5:O13" si="2">D5-J5+O4</f>
+        <f t="shared" ref="O5:O13" si="3">D5-J5+O4</f>
         <v>1596.6000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>14</v>
       </c>
@@ -922,22 +922,22 @@
         <v>450</v>
       </c>
       <c r="J6">
-        <f>H6+I6-D21</f>
+        <f t="shared" si="1"/>
         <v>807.25</v>
       </c>
       <c r="M6" s="4">
         <v>45816</v>
       </c>
       <c r="N6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3814.3500000000004</v>
       </c>
       <c r="O6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2189.3500000000004</v>
       </c>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>15</v>
       </c>
@@ -959,22 +959,22 @@
         <v>500</v>
       </c>
       <c r="J7">
-        <f>H7+I7-D22</f>
+        <f t="shared" si="1"/>
         <v>807.25</v>
       </c>
       <c r="M7" s="4">
         <v>45846</v>
       </c>
       <c r="N7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4907.1000000000004</v>
       </c>
       <c r="O7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2782.1000000000004</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>16</v>
       </c>
@@ -996,22 +996,22 @@
         <v>500</v>
       </c>
       <c r="J8">
-        <f>H8+I8-D23</f>
+        <f t="shared" si="1"/>
         <v>807.25</v>
       </c>
       <c r="M8" s="4">
         <v>45877</v>
       </c>
       <c r="N8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5999.85</v>
       </c>
       <c r="O8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3374.8500000000004</v>
       </c>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>17</v>
       </c>
@@ -1033,22 +1033,22 @@
         <v>600</v>
       </c>
       <c r="J9">
-        <f>H9+I9-D24</f>
+        <f t="shared" si="1"/>
         <v>757.25</v>
       </c>
       <c r="M9" s="4">
         <v>45908</v>
       </c>
       <c r="N9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7242.6</v>
       </c>
       <c r="O9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4017.6000000000004</v>
       </c>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>18</v>
       </c>
@@ -1070,22 +1070,22 @@
         <v>600</v>
       </c>
       <c r="J10">
-        <f>H10+I10-D25</f>
+        <f t="shared" si="1"/>
         <v>757.25</v>
       </c>
       <c r="M10" s="4">
         <v>45938</v>
       </c>
       <c r="N10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8485.35</v>
       </c>
       <c r="O10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4660.3500000000004</v>
       </c>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>19</v>
       </c>
@@ -1107,22 +1107,22 @@
         <v>600</v>
       </c>
       <c r="J11">
-        <f>H11+I11-D26</f>
+        <f t="shared" si="1"/>
         <v>757.25</v>
       </c>
       <c r="M11" s="4">
         <v>45969</v>
       </c>
       <c r="N11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9728.1</v>
       </c>
       <c r="O11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5303.1</v>
       </c>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>20</v>
       </c>
@@ -1144,22 +1144,22 @@
         <v>600</v>
       </c>
       <c r="J12">
-        <f>H12+I12-D27</f>
+        <f t="shared" si="1"/>
         <v>757.25</v>
       </c>
       <c r="M12" s="4">
         <v>45999</v>
       </c>
       <c r="N12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10970.85</v>
       </c>
       <c r="O12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5945.85</v>
       </c>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>21</v>
       </c>
@@ -1181,22 +1181,22 @@
         <v>600</v>
       </c>
       <c r="J13">
-        <f>H13+I13-D28</f>
+        <f t="shared" si="1"/>
         <v>757.25</v>
       </c>
       <c r="M13" s="4">
         <v>46030</v>
       </c>
       <c r="N13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12213.6</v>
       </c>
       <c r="O13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6588.6</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="45">
+    <row r="16" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>22</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>10</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>420.63</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" ref="H17:H28" si="3">SUM(C17:G17)</f>
+        <f t="shared" ref="H17:H28" si="4">SUM(C17:G17)</f>
         <v>420.63</v>
       </c>
       <c r="K17" t="s">
@@ -1255,11 +1255,11 @@
         <v>101.99</v>
       </c>
       <c r="N17" s="5">
-        <f t="shared" ref="N17:N28" si="4">SUM(K17:M17)</f>
+        <f t="shared" ref="N17:N28" si="5">SUM(K17:M17)</f>
         <v>394.71000000000004</v>
       </c>
     </row>
-    <row r="18" spans="2:14">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>11</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>57.25</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>208.94</v>
       </c>
       <c r="K18" t="s">
@@ -1287,11 +1287,11 @@
         <v>86.4</v>
       </c>
       <c r="N18" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>86.4</v>
       </c>
     </row>
-    <row r="19" spans="2:14">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>12</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>57.25</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>232.25</v>
       </c>
       <c r="K19" t="s">
@@ -1318,11 +1318,11 @@
         <v>200</v>
       </c>
       <c r="N19" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>13</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>57.25</v>
       </c>
       <c r="H20" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>157.25</v>
       </c>
       <c r="K20" t="s">
@@ -1349,11 +1349,11 @@
         <v>200</v>
       </c>
       <c r="N20" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>14</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>57.25</v>
       </c>
       <c r="H21" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>157.25</v>
       </c>
       <c r="K21" t="s">
@@ -1379,11 +1379,11 @@
         <v>200</v>
       </c>
       <c r="N21" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>15</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>57.25</v>
       </c>
       <c r="H22" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>157.25</v>
       </c>
       <c r="K22" t="s">
@@ -1409,11 +1409,11 @@
         <v>150</v>
       </c>
       <c r="N22" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="2:14">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>16</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>57.25</v>
       </c>
       <c r="H23" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>157.25</v>
       </c>
       <c r="K23" t="s">
@@ -1439,11 +1439,11 @@
         <v>150</v>
       </c>
       <c r="N23" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="2:14">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>17</v>
       </c>
@@ -1458,18 +1458,18 @@
         <v>57.25</v>
       </c>
       <c r="H24" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>157.25</v>
       </c>
       <c r="K24" t="s">
         <v>17</v>
       </c>
       <c r="N24" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>18</v>
       </c>
@@ -1484,18 +1484,18 @@
         <v>57.25</v>
       </c>
       <c r="H25" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>157.25</v>
       </c>
       <c r="K25" t="s">
         <v>18</v>
       </c>
       <c r="N25" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>19</v>
       </c>
@@ -1510,18 +1510,18 @@
         <v>57.25</v>
       </c>
       <c r="H26" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>157.25</v>
       </c>
       <c r="K26" t="s">
         <v>19</v>
       </c>
       <c r="N26" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>20</v>
       </c>
@@ -1536,18 +1536,18 @@
         <v>57.25</v>
       </c>
       <c r="H27" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>157.25</v>
       </c>
       <c r="K27" t="s">
         <v>20</v>
       </c>
       <c r="N27" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>21</v>
       </c>
@@ -1562,18 +1562,18 @@
         <v>57.25</v>
       </c>
       <c r="H28" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>157.25</v>
       </c>
       <c r="K28" t="s">
         <v>21</v>
       </c>
       <c r="N28" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" ht="45">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>30</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="2:14">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D32">
         <f>780/2</f>
         <v>390</v>
@@ -1621,7 +1621,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>26</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D36">
         <v>9.99</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="64" s="2" customFormat="1" ht="45" customHeight="1"/>
+    <row r="64" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <customProperties>
@@ -1689,15 +1689,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E62B397F05B5E5438624A65F15F35860" ma:contentTypeVersion="6" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="0d363647826d2362d0394f045227ee98">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="006878da-32b6-418e-a21e-40a53b773589" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ec43d7baba61d48b83411989d341fec" ns3:_="">
     <xsd:import namespace="006878da-32b6-418e-a21e-40a53b773589"/>
@@ -1853,14 +1844,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1965E4C-1BC7-4444-922C-B87B2F73010A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1965E4C-1BC7-4444-922C-B87B2F73010A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="006878da-32b6-418e-a21e-40a53b773589"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED11C3C3-F614-4137-A094-C088703CCB0A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD2DB61A-C801-4FC3-ABE3-9869E6A70950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="006878da-32b6-418e-a21e-40a53b773589"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD2DB61A-C801-4FC3-ABE3-9869E6A70950}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED11C3C3-F614-4137-A094-C088703CCB0A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>